<commit_message>
till ctx merging done
</commit_message>
<xml_diff>
--- a/public/bulk-tray-sheet-sample.xlsx
+++ b/public/bulk-tray-sheet-sample.xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26312"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3897453-0FD2-4C26-822C-8C010959324F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240"/>
+    <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Tray-Category</t>
   </si>
@@ -41,11 +55,14 @@
   <si>
     <t>CPC</t>
   </si>
+  <si>
+    <t>Tray-Grade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -524,15 +541,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -581,6 +590,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -627,7 +644,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -659,9 +676,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -693,6 +728,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -868,45 +921,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -915,24 +971,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>